<commit_message>
added all the devices data gathering from the xlsx
</commit_message>
<xml_diff>
--- a/SampleDCMap.xlsx
+++ b/SampleDCMap.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arad\PycharmProjects\SimpliDC_Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SimpliDC\SimpliDC_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42C2CDF-B513-49F0-B0F3-01392A4BA99C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C24FD51-6CE9-451E-9760-AC9A332E79F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E9720525-B099-4735-B456-B62EF23782C1}"/>
   </bookViews>
@@ -20,15 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -252,9 +243,6 @@
     <t>Network</t>
   </si>
   <si>
-    <t>Xdevice</t>
-  </si>
-  <si>
     <t>cisco-ucs</t>
   </si>
   <si>
@@ -304,6 +292,9 @@
   </si>
   <si>
     <t>Prod</t>
+  </si>
+  <si>
+    <t>XDevice</t>
   </si>
 </sst>
 </file>
@@ -660,13 +651,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA69DFAE-4764-4D24-B30F-D4AE122A18A7}">
   <dimension ref="A1:BJ5"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="AY1" workbookViewId="0">
-      <selection activeCell="BF3" sqref="BF3"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="13" width="8.88671875" style="1"/>
+    <col min="1" max="7" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="33.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" style="1" customWidth="1"/>
+    <col min="10" max="13" width="8.88671875" style="1"/>
     <col min="14" max="14" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -864,7 +858,7 @@
         <v>57</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>58</v>
@@ -1037,19 +1031,19 @@
         <v>70</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>59</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>61</v>
@@ -1079,7 +1073,7 @@
         <v>61</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T3" s="1" t="b">
         <v>0</v>
@@ -1088,10 +1082,10 @@
         <v>61</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>64</v>
@@ -1213,19 +1207,19 @@
         <v>71</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>59</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>61</v>
@@ -1255,7 +1249,7 @@
         <v>61</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="T4" s="1" t="b">
         <v>0</v>
@@ -1386,22 +1380,22 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>59</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>61</v>

</xml_diff>